<commit_message>
update ELB target instances
</commit_message>
<xml_diff>
--- a/template_resource.xlsx
+++ b/template_resource.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA75D1B-1507-4A77-95A2-6AE76B48F6A5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2B2715-7585-4ADA-855B-BC1A5DF5E721}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="infomation" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
   <si>
     <t>Security Group ID</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>Rule condition Field</t>
+  </si>
+  <si>
+    <t>Target Group VPC ID</t>
+  </si>
+  <si>
+    <t>Target Instances</t>
   </si>
 </sst>
 </file>
@@ -285,7 +291,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -386,11 +392,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -414,6 +433,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -447,7 +467,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -730,7 +750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70181BC-1538-4460-92B0-5D516F290EEC}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -744,104 +764,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -889,13 +909,13 @@
       <c r="E17" s="11"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
@@ -1147,28 +1167,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="20" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="19"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="20"/>
       <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1590,24 +1610,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="23"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="12" t="s">
         <v>44</v>
       </c>
@@ -1628,10 +1648,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DFB7C1C-74A7-44F1-B0C5-B05D8EEE85AD}">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1652,60 +1672,68 @@
     <col min="14" max="14" width="33.5703125" customWidth="1"/>
     <col min="15" max="15" width="27" customWidth="1"/>
     <col min="16" max="16" width="23.28515625" customWidth="1"/>
-    <col min="17" max="17" width="17.28515625" customWidth="1"/>
+    <col min="17" max="17" width="24.85546875" customWidth="1"/>
+    <col min="18" max="18" width="17.28515625" customWidth="1"/>
+    <col min="19" max="19" width="50.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="L1" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="M1" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="N1" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="O1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="P1" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="Q1" s="24" t="s">
+      <c r="Q1" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="R1" s="25" t="s">
         <v>61</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>